<commit_message>
Mejoras en la creación de puntos de venta y monitores de cocina
</commit_message>
<xml_diff>
--- a/projects/Prueba2/salida.xlsx
+++ b/projects/Prueba2/salida.xlsx
@@ -1507,17 +1507,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>6624</t>
+          <t>8594</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>6624</t>
+          <t>8594</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>:R=OArVo9Y</t>
+          <t>5DoJ4D?Iu-</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -1532,7 +1532,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\usuarios\Usuario-Infogral.png</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\usuarios\Usuario-Infogral.png</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -1567,17 +1567,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1271</t>
+          <t>7618</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>5259</t>
+          <t>8881</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Vt|nXe1[Aavq</t>
+          <t>Yy1&gt;0N}R</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -1592,7 +1592,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\usuarios\Administrador.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\usuarios\Administrador.jpg</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -1627,12 +1627,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>6892</t>
+          <t>2577</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0131</t>
+          <t>8774</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1652,7 +1652,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\usuarios\Encargado.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\usuarios\Encargado.jpg</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -1687,12 +1687,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>5001</t>
+          <t>4850</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1403</t>
+          <t>0208</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -1707,7 +1707,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\usuarios\Camarero.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\usuarios\Camarero.jpg</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -1742,12 +1742,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0480</t>
+          <t>4460</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>5814</t>
+          <t>4319</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -1762,7 +1762,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\usuarios\Camarero.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\usuarios\Camarero.jpg</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -1797,12 +1797,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>3095</t>
+          <t>1479</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>4976</t>
+          <t>4666</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -1817,7 +1817,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\usuarios\Cocinero.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\usuarios\Cocinero.jpg</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -3456,7 +3456,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\notas\con-hielo.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\notas\con-hielo.jpg</t>
         </is>
       </c>
     </row>
@@ -3488,7 +3488,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\notas\sin-hielo.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\notas\sin-hielo.jpg</t>
         </is>
       </c>
     </row>
@@ -3520,7 +3520,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\notas\con-limon.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\notas\con-limon.jpg</t>
         </is>
       </c>
     </row>
@@ -3552,7 +3552,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\notas\sin-limon.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\notas\sin-limon.jpg</t>
         </is>
       </c>
     </row>
@@ -3865,7 +3865,7 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\cavas\copa.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\cavas\copa.jpg</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
@@ -3928,7 +3928,7 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\cavas\botella.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\cavas\botella.jpg</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
@@ -4054,7 +4054,7 @@
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\cavas\copa.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\cavas\copa.jpg</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\cavas\botella.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\cavas\botella.jpg</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
@@ -4243,7 +4243,7 @@
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\cavas\copa.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\cavas\copa.jpg</t>
         </is>
       </c>
       <c r="X9" t="inlineStr">
@@ -4306,7 +4306,7 @@
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\cavas\botella.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\cavas\botella.jpg</t>
         </is>
       </c>
       <c r="X10" t="inlineStr">
@@ -4571,7 +4571,7 @@
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\hamburgueseria\pizza-margarita.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\hamburgueseria\pizza-margarita.jpg</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
@@ -4644,7 +4644,7 @@
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\aguas\agua-con-gas.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\aguas\agua-con-gas.jpg</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
@@ -4718,7 +4718,7 @@
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\refrescos\coca-cola-1.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\refrescos\coca-cola-1.jpg</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
@@ -4792,7 +4792,7 @@
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\refrescos\cola-zero.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\refrescos\cola-zero.jpg</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
@@ -4866,7 +4866,7 @@
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\refrescos\fanta-limon.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\refrescos\fanta-limon.jpg</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
@@ -4940,7 +4940,7 @@
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\refrescos\fanta-naranja.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\refrescos\fanta-naranja.jpg</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
@@ -5014,7 +5014,7 @@
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\refrescos\ginger-ale.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\refrescos\ginger-ale.jpg</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\refrescos\pepsi-normal.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\refrescos\pepsi-normal.jpg</t>
         </is>
       </c>
       <c r="V21" t="inlineStr">
@@ -5162,7 +5162,7 @@
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\refrescos\redbull.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\refrescos\redbull.jpg</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
@@ -5236,7 +5236,7 @@
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\vodkas\absolut.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\vodkas\absolut.jpg</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
@@ -5306,7 +5306,7 @@
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\vodkas\chupito.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\vodkas\chupito.jpg</t>
         </is>
       </c>
       <c r="X24" t="inlineStr">
@@ -5369,7 +5369,7 @@
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\vodkas\copa.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\vodkas\copa.jpg</t>
         </is>
       </c>
       <c r="X25" t="inlineStr">
@@ -5432,7 +5432,7 @@
       </c>
       <c r="U26" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\vodkas\botella.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\vodkas\botella.jpg</t>
         </is>
       </c>
       <c r="X26" t="inlineStr">
@@ -5493,7 +5493,7 @@
       </c>
       <c r="U27" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\vodkas\beluga.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\vodkas\beluga.jpg</t>
         </is>
       </c>
       <c r="V27" t="inlineStr">
@@ -5563,7 +5563,7 @@
       </c>
       <c r="U28" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\vodkas\chupito.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\vodkas\chupito.jpg</t>
         </is>
       </c>
       <c r="X28" t="inlineStr">
@@ -5626,7 +5626,7 @@
       </c>
       <c r="U29" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\vodkas\copa.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\vodkas\copa.jpg</t>
         </is>
       </c>
       <c r="X29" t="inlineStr">
@@ -5689,7 +5689,7 @@
       </c>
       <c r="U30" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\vodkas\botella.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\vodkas\botella.jpg</t>
         </is>
       </c>
       <c r="X30" t="inlineStr">
@@ -5750,7 +5750,7 @@
       </c>
       <c r="U31" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\vodkas\belvedere.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\vodkas\belvedere.jpg</t>
         </is>
       </c>
       <c r="V31" t="inlineStr">
@@ -5820,7 +5820,7 @@
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\vodkas\chupito.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\vodkas\chupito.jpg</t>
         </is>
       </c>
       <c r="X32" t="inlineStr">
@@ -5883,7 +5883,7 @@
       </c>
       <c r="U33" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\vodkas\copa.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\vodkas\copa.jpg</t>
         </is>
       </c>
       <c r="X33" t="inlineStr">
@@ -5946,7 +5946,7 @@
       </c>
       <c r="U34" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\vodkas\botella.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\vodkas\botella.jpg</t>
         </is>
       </c>
       <c r="X34" t="inlineStr">
@@ -6007,7 +6007,7 @@
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\vodkas\ciroc.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\vodkas\ciroc.jpg</t>
         </is>
       </c>
       <c r="V35" t="inlineStr">
@@ -6077,7 +6077,7 @@
       </c>
       <c r="U36" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\vodkas\chupito.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\vodkas\chupito.jpg</t>
         </is>
       </c>
       <c r="X36" t="inlineStr">
@@ -6140,7 +6140,7 @@
       </c>
       <c r="U37" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\vodkas\copa.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\vodkas\copa.jpg</t>
         </is>
       </c>
       <c r="X37" t="inlineStr">
@@ -6203,7 +6203,7 @@
       </c>
       <c r="U38" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\vodkas\botella.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\vodkas\botella.jpg</t>
         </is>
       </c>
       <c r="X38" t="inlineStr">
@@ -6264,7 +6264,7 @@
       </c>
       <c r="U39" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\vodkas\smirnoff-red-vodka.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\vodkas\smirnoff-red-vodka.jpg</t>
         </is>
       </c>
       <c r="V39" t="inlineStr">
@@ -6334,7 +6334,7 @@
       </c>
       <c r="U40" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\vodkas\chupito.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\vodkas\chupito.jpg</t>
         </is>
       </c>
       <c r="X40" t="inlineStr">
@@ -6397,7 +6397,7 @@
       </c>
       <c r="U41" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\vodkas\copa.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\vodkas\copa.jpg</t>
         </is>
       </c>
       <c r="X41" t="inlineStr">
@@ -6460,7 +6460,7 @@
       </c>
       <c r="U42" t="inlineStr">
         <is>
-          <t>C:\Users\Nest\Desktop\infogral\dist-maker (local)\en-desarrollo\imagenesAgora\vodkas\botella.jpg</t>
+          <t>C:\Users\nesto\Desktop\Agora_LAB\imagenesAgora\vodkas\botella.jpg</t>
         </is>
       </c>
       <c r="X42" t="inlineStr">

</xml_diff>